<commit_message>
Set minimum threshold for data count 3
</commit_message>
<xml_diff>
--- a/textToOps/data/raw/op_type.xlsx
+++ b/textToOps/data/raw/op_type.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,7 +555,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>data queries,geometry measurement,data queries</t>
+          <t>data queries,geometry measurement,data queries,vegetation 애매함. osm만으로 불가.</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -594,7 +594,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>data queries,buffer,buffer,overlay analysis,overlay analysis</t>
+          <t>topography,data model conversion,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -607,7 +607,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>data queries,overlay analysis</t>
+          <t>data queries,buffer,buffer,overlay analysis,overlay analysis,two set of geometries</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -620,7 +620,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>data editing,data queries,network analysis,classification,data queries,overlay analysis,data queries,overlay analysis,data queries,overlay analysis</t>
+          <t>data queries,overlay analysis</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -633,7 +633,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>data queries,network analysis,data queries,network analysis,classification,data queries,overlay analysis</t>
+          <t>data editing,data queries,network analysis,classification,data queries,overlay analysis,data queries,overlay analysis,data queries,overlay analysis</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -646,7 +646,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries,overlay analysis,data queries,overlay analysis</t>
+          <t>data queries,buffer,overlay analysis,정확히 카메라가 무엇을 뜻하는가</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -659,7 +659,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>data editing,data queries,buffer,overlay analysis</t>
+          <t>data queries,buffer,overlay analysis,각자 buffer를 union 해야하네</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -672,7 +672,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>topography,classification,data queries,data model conversion,overlay analysis</t>
+          <t>data queries,buffer,overlay analysis,matter of scale. 도로는 line인가</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -685,7 +685,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>data queries,geometry measurement,data editing,data queries</t>
+          <t>data queries,buffer,overlay analysis,major가 무엇인지</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -698,7 +698,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>geostatistics  ,classification,data queries,data model conversion,overlay analysis</t>
+          <t>data queries,network analysis,data queries,network analysis,classification,data queries,overlay analysis,어디로 부터 가장 가까운 소방서</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -711,7 +711,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries,overlay analysis</t>
+          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries,overlay analysis,data queries,overlay analysis</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -724,7 +724,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis,data queries</t>
+          <t>data queries,buffer,overlay analysis,shop이 너무나 많다</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -737,7 +737,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>network analysis,data queries,buffer,overlay analysis,data queries</t>
+          <t>data editing,data queries,buffer,overlay analysis</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -750,7 +750,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>overlay analysis,topography</t>
+          <t>data editing,data queries,buffer,overlay analysis,what area는 그냥 boundary만 얘기하는 것인가? 아니면 다른 attribute도 clip하라는 것인가. 일단 clip. urban tag를 그렇게 사용하지도 않는다</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -763,7 +763,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>data queries,overlay analysis,data editing,data queries</t>
+          <t>topography,classification,data queries,data model conversion,overlay analysis</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -776,7 +776,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>data editing,data queries,overlay analysis,data editing,data queries</t>
+          <t>data queries,geometry measurement,data editing,data queries</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -789,7 +789,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>data editing,overlay analysis,data editing,data queries</t>
+          <t>geostatistics  ,classification,data queries,data model conversion,overlay analysis</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -802,7 +802,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>data editing,data queries,data editing</t>
+          <t>data queries,network analysis,classification,data queries,overlay analysis,data queries,overlay analysis</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -815,7 +815,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,generalization,geostatistics  </t>
+          <t>data queries,buffer,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -828,7 +828,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t xml:space="preserve">data editing,data queries,generalization,geostatistics  </t>
+          <t>network analysis,data queries,buffer,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -841,7 +841,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>data editing,overlay analysis,data queries</t>
+          <t>data queries,overlay analysis,data queries,osm urban이 있긴 하지만 거의 안쓴다</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -854,7 +854,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t xml:space="preserve">data editing,data queries,geostatistics  </t>
+          <t>overlay analysis,topography</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -867,7 +867,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,geostatistics  </t>
+          <t>data queries,overlay analysis,data editing,data queries</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -880,7 +880,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>data editing,data queries,overlay analysis,data editing</t>
+          <t>data editing,data queries,overlay analysis,data editing,data queries</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -893,7 +893,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>data editing,data queries,network analysis,data queries</t>
+          <t>data editing,overlay analysis,data editing,data queries</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -906,7 +906,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t xml:space="preserve">data queries,overlay analysis,geostatistics  </t>
+          <t>data editing,data queries,data editing</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -919,7 +919,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>data queries,network analysis</t>
+          <t>data queries,generalization,geostatistics  ,https://pro.arcgis.com/en/pro-app/latest/tool-reference/spatial-statistics/h-how-central-feature-spatial-statistics-works.htm</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -932,7 +932,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>data queries,buffer,overlay analysis,data queries,geometry measurement,data queries</t>
+          <t xml:space="preserve">data editing,data queries,generalization,geostatistics  </t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -945,7 +945,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>data queries,buffer,buffer,buffer,overlay analysis,overlay analysis,overlay analysis,geometry measurement,data queries,geometry measurement,data queries,geometry measurement,data queries</t>
+          <t xml:space="preserve">data queries,generalization,geostatistics  </t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -958,7 +958,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>data queries,geometry measurement,data queries,buffer,overlay analysis,data queries</t>
+          <t>data editing,overlay analysis,data queries</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -971,11 +971,193 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>geocoding,data queries,network analysis,data queries</t>
+          <t xml:space="preserve">data editing,data queries,geostatistics  </t>
         </is>
       </c>
       <c r="C42" t="n">
         <v>40</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">data queries,geostatistics  </t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>data editing,data queries,overlay analysis,data editing</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>data editing,data queries,network analysis,data queries</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">data queries,overlay analysis,geostatistics  </t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>data queries,network analysis</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>data editing,buffer,overlay analysis,data editing,data queries</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>data queries,geometry measurement,data queries</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>data queries,overlay analysis,data queries,어디선 polygon, 어디선 linestring</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>data queries,geometry measurement,data queries,https://wiki.openstreetmap.org/wiki/sparql_examples</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>data queries,buffer,overlay analysis,data queries,geometry measurement,data queries</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>data queries,buffer,buffer,buffer,overlay analysis,overlay analysis,overlay analysis,geometry measurement,data queries,geometry measurement,data queries,geometry measurement,data queries</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>data queries,geometry measurement,data queries,buffer,overlay analysis,data queries</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>data queries,network analysis,data queries,network analysis,classification,data queries,overlay analysis</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>geocoding,data queries,network analysis,data queries,멘탈 헬스를 누가 담당할건데…</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>